<commit_message>
Added task to ID-1
</commit_message>
<xml_diff>
--- a/User_stories.xlsx
+++ b/User_stories.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26101"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26505"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srinu_akkineni/Desktop/SoftHouse/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Desktop/Team-1/Skill_DB/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Login</t>
   </si>
   <si>
-    <t>As a user, I want to login to the system. Here, user can be line manager, site manager and employee.</t>
-  </si>
-  <si>
     <t>Site Manager Login</t>
   </si>
   <si>
@@ -128,6 +125,12 @@
   </si>
   <si>
     <t>As a user, I should be able to know the number of employees, site mangers and line managers for each site</t>
+  </si>
+  <si>
+    <t>As a user, I want to login to the system. Here, user can be line manager, site manager or employee.</t>
+  </si>
+  <si>
+    <t>Is to create a webpage using bootstrap and AngularJS containing two input fields (UserName and PassWord), two buttons (Register and LogIn), a Remember me check box</t>
   </si>
 </sst>
 </file>
@@ -547,12 +550,13 @@
   <dimension ref="B1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="42.6640625" customWidth="1"/>
+    <col min="6" max="6" width="30.33203125" customWidth="1"/>
     <col min="10" max="10" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -584,7 +588,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" ht="106" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2">
         <v>1</v>
@@ -593,9 +597,11 @@
         <v>11</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -607,10 +613,10 @@
         <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -627,7 +633,7 @@
         <v>8</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -644,7 +650,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -661,7 +667,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -674,10 +680,10 @@
         <v>6</v>
       </c>
       <c r="D8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>15</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="26" x14ac:dyDescent="0.2">
@@ -685,10 +691,10 @@
         <v>7</v>
       </c>
       <c r="D9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>17</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="26" x14ac:dyDescent="0.2">
@@ -696,10 +702,10 @@
         <v>8</v>
       </c>
       <c r="D10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="26" x14ac:dyDescent="0.2">
@@ -707,10 +713,10 @@
         <v>9</v>
       </c>
       <c r="D11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="26" x14ac:dyDescent="0.2">
@@ -718,10 +724,10 @@
         <v>10</v>
       </c>
       <c r="D12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="26" x14ac:dyDescent="0.2">
@@ -729,10 +735,10 @@
         <v>11</v>
       </c>
       <c r="D13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>28</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="26" x14ac:dyDescent="0.2">
@@ -740,10 +746,10 @@
         <v>12</v>
       </c>
       <c r="D14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="9" t="s">
         <v>30</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="39" x14ac:dyDescent="0.2">
@@ -751,10 +757,10 @@
         <v>13</v>
       </c>
       <c r="D15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>32</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>